<commit_message>
update to alice latest dicts
</commit_message>
<xml_diff>
--- a/inst/extdata/Cleaning_dict_alice.xlsx
+++ b/inst/extdata/Cleaning_dict_alice.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aljc201/Desktop/covidmonitor/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DCF3BE-771D-7244-9431-A3A702548609}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9695C9EF-67ED-8A4C-B6D2-076FAFFD92D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29120" yWindow="3540" windowWidth="19840" windowHeight="16060" activeTab="2" xr2:uid="{057372D8-FD55-424B-B3E3-F97E8D1F1A18}"/>
+    <workbookView xWindow="10840" yWindow="10680" windowWidth="34600" windowHeight="16060" xr2:uid="{057372D8-FD55-424B-B3E3-F97E8D1F1A18}"/>
   </bookViews>
   <sheets>
-    <sheet name="hcw" sheetId="1" r:id="rId1"/>
-    <sheet name="yesno" sheetId="5" r:id="rId2"/>
-    <sheet name="ncd" sheetId="6" r:id="rId3"/>
-    <sheet name="capital" sheetId="7" r:id="rId4"/>
-    <sheet name="confirmed" sheetId="8" r:id="rId5"/>
+    <sheet name="all_clean" sheetId="9" r:id="rId1"/>
+    <sheet name="capital" sheetId="7" r:id="rId2"/>
+    <sheet name="confirmed" sheetId="8" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="372">
   <si>
     <t>HYGIENE</t>
   </si>
@@ -628,9 +626,6 @@
     <t>vasculaire</t>
   </si>
   <si>
-    <t>(?i)^N$</t>
-  </si>
-  <si>
     <t>foie</t>
   </si>
   <si>
@@ -661,18 +656,6 @@
     <t>nil</t>
   </si>
   <si>
-    <t>(?i)^no$</t>
-  </si>
-  <si>
-    <t>(?i)^nil$</t>
-  </si>
-  <si>
-    <t>(?i)^none$</t>
-  </si>
-  <si>
-    <t>(?i)^non$</t>
-  </si>
-  <si>
     <t>ht</t>
   </si>
   <si>
@@ -703,18 +686,6 @@
     <t>glaucom</t>
   </si>
   <si>
-    <t>(?i)^rien$</t>
-  </si>
-  <si>
-    <t>(?i)^rien a signaler$</t>
-  </si>
-  <si>
-    <t>(?i)^rien a signale$</t>
-  </si>
-  <si>
-    <t>(?i)^Sans particularite$</t>
-  </si>
-  <si>
     <t>rhum</t>
   </si>
   <si>
@@ -1118,6 +1089,60 @@
   </si>
   <si>
     <t>pressure,</t>
+  </si>
+  <si>
+    <t>not_occupation</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>imported</t>
+  </si>
+  <si>
+    <t>nn</t>
+  </si>
+  <si>
+    <t>know</t>
+  </si>
+  <si>
+    <t>unknown_sympt</t>
+  </si>
+  <si>
+    <t>Not Known</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Not provided</t>
+  </si>
+  <si>
+    <t>Not Available</t>
+  </si>
+  <si>
+    <t>not_indicated</t>
+  </si>
+  <si>
+    <t>Not given</t>
+  </si>
+  <si>
+    <t>Not avaliable</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>Not Available;</t>
+  </si>
+  <si>
+    <t>sickle</t>
   </si>
 </sst>
 </file>
@@ -1498,176 +1523,1058 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{384F988A-E9AB-624F-A3E4-2D041F636D11}">
-  <dimension ref="A1:A32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{092CE1D0-0E52-5D44-9DBC-8794A4E177B7}">
+  <dimension ref="A1:AB82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:28" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" t="s">
+        <v>224</v>
+      </c>
+      <c r="O2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>93</v>
+      </c>
+      <c r="R2" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" t="s">
+        <v>95</v>
+      </c>
+      <c r="T2" t="s">
+        <v>112</v>
+      </c>
+      <c r="U2" t="s">
+        <v>98</v>
+      </c>
+      <c r="V2" t="s">
+        <v>133</v>
+      </c>
+      <c r="W2" t="s">
+        <v>100</v>
+      </c>
+      <c r="X2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" t="s">
+        <v>207</v>
+      </c>
+      <c r="O3" t="s">
+        <v>227</v>
+      </c>
+      <c r="P3" t="s">
+        <v>347</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>151</v>
+      </c>
+      <c r="R3" t="s">
+        <v>113</v>
+      </c>
+      <c r="S3" t="s">
+        <v>116</v>
+      </c>
+      <c r="T3" t="s">
+        <v>192</v>
+      </c>
+      <c r="U3" t="s">
+        <v>110</v>
+      </c>
+      <c r="V3" t="s">
+        <v>136</v>
+      </c>
+      <c r="W3" t="s">
+        <v>176</v>
+      </c>
+      <c r="X3" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" t="s">
+        <v>73</v>
+      </c>
+      <c r="N4" t="s">
+        <v>225</v>
+      </c>
+      <c r="O4" t="s">
+        <v>214</v>
+      </c>
+      <c r="P4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="U4" t="s">
+        <v>115</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="W4" t="s">
+        <v>202</v>
+      </c>
+      <c r="X4" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>342</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>214</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2"/>
+      <c r="C5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5" t="s">
+        <v>206</v>
+      </c>
+      <c r="O5" t="s">
+        <v>228</v>
+      </c>
+      <c r="P5" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>348</v>
+      </c>
+      <c r="R5" t="s">
+        <v>182</v>
+      </c>
+      <c r="T5" t="s">
+        <v>175</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="W5" t="s">
+        <v>220</v>
+      </c>
+      <c r="X5" t="s">
+        <v>371</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>231</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" t="s">
+        <v>208</v>
+      </c>
+      <c r="O6" t="s">
+        <v>230</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="T6" t="s">
+        <v>346</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>344</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C7" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" t="s">
+        <v>226</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N8" t="s">
+        <v>229</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="R9" t="s">
+        <v>353</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E10" t="s">
+        <v>39</v>
+      </c>
+      <c r="N10" t="s">
+        <v>300</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="N11" t="s">
+        <v>358</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" t="s">
+        <v>85</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="N13" t="s">
+        <v>359</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB16" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB17" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB18" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB19" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E20" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB20" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB21" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB22" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB23" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB24" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB25" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB26" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB27" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB28" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB29" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB30" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="AB31" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>82</v>
+      </c>
+      <c r="AB32" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB33" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB34" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB35" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB36" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB37" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB38" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB39" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB40" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB41" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="42" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB42" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB43" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB44" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="45" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB45" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB46" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB47" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB48" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB49" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="50" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB50" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="51" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB51" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB52" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB53" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB54" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB55" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB56" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="57" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB57" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="58" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB58" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB59" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB60" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB61" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="62" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB62" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB63" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB64" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="65" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB65" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="66" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB66" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="67" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB67" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="68" spans="28:28" ht="16" x14ac:dyDescent="0.2">
+      <c r="AB68" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB69" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="70" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB70" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="71" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB71" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="72" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB72" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="73" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB73" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="74" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB74" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB75" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="76" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB76" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="77" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB77" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="78" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB78" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="79" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB79" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="80" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB80" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="81" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB81" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="82" spans="28:28" x14ac:dyDescent="0.2">
+      <c r="AB82" s="2" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -1676,1268 +2583,277 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABFBA860-4121-CE46-8A10-A094F9DB7896}">
-  <dimension ref="A1:L22"/>
-  <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>349</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>349</v>
-      </c>
-      <c r="D2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="J2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" t="s">
-        <v>233</v>
-      </c>
-      <c r="L2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K3" t="s">
-        <v>208</v>
-      </c>
-      <c r="L3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G4" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" t="s">
-        <v>70</v>
-      </c>
-      <c r="J4" t="s">
-        <v>73</v>
-      </c>
-      <c r="K4" t="s">
-        <v>234</v>
-      </c>
-      <c r="L4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G5" t="s">
-        <v>87</v>
-      </c>
-      <c r="H5" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" t="s">
-        <v>71</v>
-      </c>
-      <c r="J5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" t="s">
-        <v>207</v>
-      </c>
-      <c r="L5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" t="s">
-        <v>209</v>
-      </c>
-      <c r="L6" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>76</v>
-      </c>
-      <c r="K7" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>83</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BE1511-0DCA-9F44-BBE3-644DD7DAA460}">
-  <dimension ref="A1:N82"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J2" t="s">
-        <v>160</v>
-      </c>
-      <c r="K2" t="s">
-        <v>166</v>
-      </c>
-      <c r="L2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M2" t="s">
-        <v>106</v>
-      </c>
-      <c r="N2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>356</v>
-      </c>
-      <c r="B3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" t="s">
-        <v>192</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H3" t="s">
-        <v>176</v>
-      </c>
-      <c r="I3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J3" t="s">
-        <v>109</v>
-      </c>
-      <c r="K3" t="s">
-        <v>202</v>
-      </c>
-      <c r="L3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="N3" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="H4" t="s">
-        <v>203</v>
-      </c>
-      <c r="I4" t="s">
-        <v>156</v>
-      </c>
-      <c r="J4" t="s">
-        <v>111</v>
-      </c>
-      <c r="K4" t="s">
-        <v>351</v>
-      </c>
-      <c r="L4" t="s">
-        <v>219</v>
-      </c>
-      <c r="M4" t="s">
-        <v>118</v>
-      </c>
-      <c r="N4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" t="s">
-        <v>357</v>
-      </c>
-      <c r="C5" t="s">
-        <v>182</v>
-      </c>
-      <c r="E5" t="s">
-        <v>175</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="H5" t="s">
-        <v>229</v>
-      </c>
-      <c r="J5" t="s">
-        <v>194</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="L5" t="s">
-        <v>240</v>
-      </c>
-      <c r="M5" t="s">
-        <v>119</v>
-      </c>
-      <c r="N5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C6" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="E6" t="s">
-        <v>355</v>
-      </c>
-      <c r="J6" t="s">
-        <v>197</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="L6" t="s">
-        <v>353</v>
-      </c>
-      <c r="M6" t="s">
-        <v>121</v>
-      </c>
-      <c r="N6" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C7" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="J7" t="s">
-        <v>201</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="M7" t="s">
-        <v>122</v>
-      </c>
-      <c r="N7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C8" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="M8" t="s">
-        <v>123</v>
-      </c>
-      <c r="N8" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>362</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="M9" t="s">
-        <v>124</v>
-      </c>
-      <c r="N9" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="K10" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M11" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M12" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M13" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M14" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M15" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M16" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M17" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M18" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M19" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M20" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M21" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M22" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M23" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M24" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="25" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M25" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="26" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M26" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="27" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M27" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="28" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M28" s="2" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="29" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M29" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M30" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="31" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M31" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M32" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M33" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M34" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="35" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M35" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M36" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="37" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M37" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="38" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M38" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="39" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M39" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="40" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M40" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M41" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="42" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M42" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="43" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M43" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="44" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M44" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="45" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M45" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M46" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="47" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M47" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="48" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M48" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M49" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M50" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="51" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M51" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M52" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="53" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M53" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="54" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M54" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="55" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M55" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M56" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="57" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M57" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="58" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M58" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="59" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M59" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="60" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M60" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="61" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M61" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="62" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M62" s="2" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="63" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M63" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="64" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M64" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="65" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M65" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="66" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M66" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="67" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M67" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="68" spans="13:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="M68" s="5" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="69" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M69" s="2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="70" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M70" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="71" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M71" s="2" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="72" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M72" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="73" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M73" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="74" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M74" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="75" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M75" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="76" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M76" s="2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="77" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M77" s="2" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="78" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M78" s="2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="79" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M79" s="2" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="80" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M80" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="81" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M81" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="82" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M82" s="2" t="s">
-        <v>358</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC8EFF2D-F821-E342-BE80-698EC0819BB7}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C2" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B3" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C3" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="C5" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B6" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="C6" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B7" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C7" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C8" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B9" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C9" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B10" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C10" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B11" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="C11" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C12" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="B13" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="C13" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B14" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C14" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B15" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B16" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C16" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="B17" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C17" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B18" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="C18" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B19" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C19" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B20" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="C20" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B21" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C21" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B22" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C22" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B23" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="C23" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B24" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C24" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2948,7 +2864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62F8E3E-3802-3F43-A0BC-8693C28A06B2}">
   <dimension ref="A1:D38"/>
   <sheetViews>
@@ -2960,330 +2876,330 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B1" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C1" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="D1" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="B2" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="B3" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B6" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="B7" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B8" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B9" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C9" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D9" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B10" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="B12" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="B13" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B14" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B15" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="B16" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="B17" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B18" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B19" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>314</v>
+      </c>
+      <c r="B20" t="s">
         <v>323</v>
-      </c>
-      <c r="B20" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="B21" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B22" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B23" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="B24" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C24" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="D24" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="B25" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B26" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="B27" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="B28" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="B29" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B30" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B31" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="B32" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B33" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>319</v>
+      </c>
+      <c r="B34" t="s">
         <v>328</v>
-      </c>
-      <c r="B34" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B35" t="s">
+        <v>328</v>
+      </c>
+      <c r="C35" t="s">
         <v>337</v>
       </c>
-      <c r="C35" t="s">
-        <v>346</v>
-      </c>
       <c r="D35" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="B36" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="B37" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="B38" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>